<commit_message>
Adding final data collection as shown in tutorial
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vheimsba\Documents\Foredrag\Semantiske teknologier\KGC\KGC22 OTTR masterclass\demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vheimsba\Documents\Foredrag\Semantiske teknologier\KGC\git\ottr-masterclass\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226B1C90-347D-416A-A87D-D3D573C075D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E7A73E-CD21-48F9-8288-5F2B0627A9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="3390" windowWidth="16200" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="satellites" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="496">
   <si>
     <t>planet</t>
   </si>
@@ -1521,9 +1521,6 @@
   </si>
   <si>
     <t>Pluto@@en</t>
-  </si>
-  <si>
-    <t>text+</t>
   </si>
 </sst>
 </file>
@@ -1914,7 +1911,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1937,7 +1934,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1960,7 +1957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1983,7 +1980,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -2006,7 +2003,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -2029,7 +2026,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -2052,7 +2049,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -2075,7 +2072,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -2098,7 +2095,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -2121,7 +2118,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -2144,7 +2141,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -2167,7 +2164,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -2190,7 +2187,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -2213,7 +2210,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -2236,7 +2233,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -2259,7 +2256,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
@@ -2282,7 +2279,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -2305,7 +2302,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -2328,7 +2325,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
@@ -2351,7 +2348,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -2374,7 +2371,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -2397,7 +2394,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
@@ -2420,7 +2417,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
@@ -2443,7 +2440,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
@@ -2466,7 +2463,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -2489,7 +2486,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -2512,7 +2509,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
@@ -2535,7 +2532,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
@@ -2558,7 +2555,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>25</v>
       </c>
@@ -2581,7 +2578,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
@@ -2604,7 +2601,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>25</v>
       </c>
@@ -2627,7 +2624,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>25</v>
       </c>
@@ -2650,7 +2647,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>25</v>
       </c>
@@ -2673,7 +2670,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>25</v>
       </c>
@@ -2696,7 +2693,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>25</v>
       </c>
@@ -2719,7 +2716,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>25</v>
       </c>
@@ -5998,7 +5995,7 @@
   <dimension ref="A1:Z1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6133,7 +6130,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -6161,7 +6158,7 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>436</v>
       </c>
@@ -6195,7 +6192,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -6239,7 +6236,7 @@
         <v>444</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>496</v>
+        <v>445</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>446</v>
@@ -6303,7 +6300,7 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="str">
         <f>CONCATENATE(":", satellites!A2)</f>
         <v>:Earth</v>
@@ -6321,7 +6318,7 @@
         <v>1737.5±0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="str">
         <f>CONCATENATE(":", satellites!A3)</f>
         <v>:Mars</v>
@@ -6339,7 +6336,7 @@
         <v>11.1±0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="str">
         <f>CONCATENATE(":", satellites!A4)</f>
         <v>:Mars</v>
@@ -6357,7 +6354,7 @@
         <v>6.2±0.18</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="str">
         <f>CONCATENATE(":", satellites!A5)</f>
         <v>:Jupiter</v>
@@ -6375,7 +6372,7 @@
         <v>1821.6±0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="str">
         <f>CONCATENATE(":", satellites!A6)</f>
         <v>:Jupiter</v>
@@ -6393,7 +6390,7 @@
         <v>1560.8±0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="str">
         <f>CONCATENATE(":", satellites!A7)</f>
         <v>:Jupiter</v>
@@ -6411,7 +6408,7 @@
         <v>2631.2±1.7</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="str">
         <f>CONCATENATE(":", satellites!A8)</f>
         <v>:Jupiter</v>
@@ -6429,7 +6426,7 @@
         <v>2410.3±1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="str">
         <f>CONCATENATE(":", satellites!A9)</f>
         <v>:Jupiter</v>
@@ -6447,7 +6444,7 @@
         <v>83.45±2.4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="str">
         <f>CONCATENATE(":", satellites!A10)</f>
         <v>:Jupiter</v>
@@ -6465,7 +6462,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="str">
         <f>CONCATENATE(":", satellites!A11)</f>
         <v>:Jupiter</v>
@@ -6483,7 +6480,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="str">
         <f>CONCATENATE(":", satellites!A12)</f>
         <v>:Jupiter</v>
@@ -6501,7 +6498,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="str">
         <f>CONCATENATE(":", satellites!A13)</f>
         <v>:Jupiter</v>
@@ -6519,7 +6516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="str">
         <f>CONCATENATE(":", satellites!A14)</f>
         <v>:Jupiter</v>
@@ -6537,7 +6534,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="str">
         <f>CONCATENATE(":", satellites!A15)</f>
         <v>:Jupiter</v>
@@ -6555,7 +6552,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="str">
         <f>CONCATENATE(":", satellites!A16)</f>
         <v>:Jupiter</v>
@@ -6573,7 +6570,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="str">
         <f>CONCATENATE(":", satellites!A17)</f>
         <v>:Jupiter</v>
@@ -6591,7 +6588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="str">
         <f>CONCATENATE(":", satellites!A18)</f>
         <v>:Jupiter</v>
@@ -6609,7 +6606,7 @@
         <v>49.3±2.0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="str">
         <f>CONCATENATE(":", satellites!A19)</f>
         <v>:Jupiter</v>
@@ -6627,7 +6624,7 @@
         <v>8.2±2.0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="str">
         <f>CONCATENATE(":", satellites!A20)</f>
         <v>:Jupiter</v>
@@ -6645,7 +6642,7 @@
         <v>21.5±2.0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="str">
         <f>CONCATENATE(":", satellites!A21)</f>
         <v>:Jupiter</v>
@@ -6663,7 +6660,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="str">
         <f>CONCATENATE(":", satellites!A22)</f>
         <v>:Jupiter</v>
@@ -6681,7 +6678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="str">
         <f>CONCATENATE(":", satellites!A23)</f>
         <v>:Jupiter</v>
@@ -6699,7 +6696,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="str">
         <f>CONCATENATE(":", satellites!A24)</f>
         <v>:Jupiter</v>
@@ -6717,7 +6714,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="str">
         <f>CONCATENATE(":", satellites!A25)</f>
         <v>:Jupiter</v>
@@ -6735,7 +6732,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="str">
         <f>CONCATENATE(":", satellites!A26)</f>
         <v>:Jupiter</v>
@@ -6753,7 +6750,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="str">
         <f>CONCATENATE(":", satellites!A27)</f>
         <v>:Jupiter</v>
@@ -6771,7 +6768,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="str">
         <f>CONCATENATE(":", satellites!A28)</f>
         <v>:Jupiter</v>
@@ -6789,7 +6786,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="str">
         <f>CONCATENATE(":", satellites!A29)</f>
         <v>:Jupiter</v>
@@ -12087,7 +12084,7 @@
       <c r="T4" s="12"/>
       <c r="U4" s="13"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -12110,7 +12107,7 @@
       <c r="T5" s="12"/>
       <c r="U5" s="13"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>436</v>
       </c>

</xml_diff>